<commit_message>
Update amplicon to also say PacBio
</commit_message>
<xml_diff>
--- a/docs/IMR-SampleSubmissionSheet_v11(LASTNAME_MMMDD).xlsx
+++ b/docs/IMR-SampleSubmissionSheet_v11(LASTNAME_MMMDD).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F64D5-CF16-4110-84AB-DB6000D6822C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27B0863-2D3D-4A70-81E2-FC53C7ADF066}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="742" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="742" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS (read first)" sheetId="3" r:id="rId1"/>
@@ -366,9 +366,6 @@
   </si>
   <si>
     <t>For client-prepared pool of amplicons (MiSeq):</t>
-  </si>
-  <si>
-    <t>For amplicon sequencing (MiSeq):</t>
   </si>
   <si>
     <r>
@@ -1280,6 +1277,9 @@
   </si>
   <si>
     <t>Integrated Microbiome Resource (IMR) Submission Template v.11 (Jul.2019)</t>
+  </si>
+  <si>
+    <t>For amplicon sequencing (MiSeq/PacBio):</t>
   </si>
 </sst>
 </file>
@@ -2149,21 +2149,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2194,15 +2237,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2227,52 +2261,18 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="14"/>
     </row>
@@ -2665,7 +2665,7 @@
     <row r="6" spans="1:2" s="85" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2683,7 +2683,7 @@
     <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2693,7 +2693,7 @@
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2723,7 +2723,7 @@
     </row>
     <row r="17" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -2761,8 +2761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,11 +2781,11 @@
       <c r="A2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="86" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
+      <c r="A3" s="98" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
@@ -2793,7 +2793,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -2802,7 +2802,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -2820,39 +2820,39 @@
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="87"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="99"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
-      <c r="B9" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" s="91"/>
+      <c r="B9" s="102" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="102"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
-      <c r="B10" s="92" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="92"/>
+      <c r="B10" s="103" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="103"/>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="101"/>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
         <v>71</v>
       </c>
       <c r="C13" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -2860,7 +2860,7 @@
         <v>72</v>
       </c>
       <c r="C14" s="80" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -2868,25 +2868,25 @@
         <v>73</v>
       </c>
       <c r="C15" s="76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="90"/>
-      <c r="C17" s="90"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="101"/>
     </row>
     <row r="18" spans="1:3" s="77" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="77" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2894,7 +2894,7 @@
         <v>72</v>
       </c>
       <c r="C19" s="81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="77" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2902,25 +2902,25 @@
         <v>73</v>
       </c>
       <c r="C20" s="76" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="16"/>
     </row>
     <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="88" t="s">
+      <c r="A22" s="100" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="88"/>
-      <c r="C22" s="88"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
     </row>
     <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="16" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="80" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -2928,7 +2928,7 @@
         <v>72</v>
       </c>
       <c r="C24" s="80" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -2936,35 +2936,35 @@
         <v>73</v>
       </c>
       <c r="C25" s="76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
     </row>
     <row r="27" spans="1:3" s="77" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="89" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="89"/>
-      <c r="C27" s="89"/>
+      <c r="A27" s="97" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
     </row>
     <row r="28" spans="1:3" s="77" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="89" t="s">
-        <v>150</v>
-      </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
+      <c r="A30" s="97" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="97"/>
+      <c r="C30" s="97"/>
     </row>
     <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="85"/>
       <c r="B31" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C31" s="85"/>
     </row>
@@ -2991,7 +2991,7 @@
   </sheetPr>
   <dimension ref="A1:AF82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3:AA14"/>
     </sheetView>
   </sheetViews>
@@ -3001,20 +3001,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
+      <c r="A1" s="111" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -3033,35 +3033,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="94"/>
+      <c r="B3" s="108"/>
       <c r="C3" s="105"/>
       <c r="D3" s="106"/>
       <c r="E3" s="106"/>
       <c r="F3" s="106"/>
       <c r="G3" s="107"/>
-      <c r="J3" s="94" t="s">
+      <c r="J3" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="117"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="117"/>
-      <c r="AA3" s="117"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -3069,35 +3069,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="94"/>
+      <c r="B4" s="108"/>
       <c r="C4" s="105"/>
       <c r="D4" s="106"/>
       <c r="E4" s="106"/>
       <c r="F4" s="106"/>
       <c r="G4" s="107"/>
-      <c r="J4" s="94" t="s">
+      <c r="J4" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="117"/>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="117"/>
-      <c r="U4" s="117"/>
-      <c r="V4" s="117"/>
-      <c r="W4" s="117"/>
-      <c r="X4" s="117"/>
-      <c r="Y4" s="117"/>
-      <c r="Z4" s="117"/>
-      <c r="AA4" s="117"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109"/>
+      <c r="X4" s="109"/>
+      <c r="Y4" s="109"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -3106,26 +3106,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="104" t="s">
+      <c r="J5" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
-      <c r="Y5" s="117"/>
-      <c r="Z5" s="117"/>
-      <c r="AA5" s="117"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="109"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="109"/>
+      <c r="Z5" s="109"/>
+      <c r="AA5" s="109"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -3133,30 +3133,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="105"/>
       <c r="D6" s="106"/>
       <c r="E6" s="106"/>
       <c r="F6" s="106"/>
       <c r="G6" s="107"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="117"/>
-      <c r="U6" s="117"/>
-      <c r="V6" s="117"/>
-      <c r="W6" s="117"/>
-      <c r="X6" s="117"/>
-      <c r="Y6" s="117"/>
-      <c r="Z6" s="117"/>
-      <c r="AA6" s="117"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="109"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="109"/>
+      <c r="V6" s="109"/>
+      <c r="W6" s="109"/>
+      <c r="X6" s="109"/>
+      <c r="Y6" s="109"/>
+      <c r="Z6" s="109"/>
+      <c r="AA6" s="109"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -3164,30 +3164,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="94"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="105"/>
       <c r="D7" s="106"/>
       <c r="E7" s="106"/>
       <c r="F7" s="106"/>
       <c r="G7" s="107"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117"/>
-      <c r="Q7" s="117"/>
-      <c r="R7" s="117"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="117"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="117"/>
-      <c r="X7" s="117"/>
-      <c r="Y7" s="117"/>
-      <c r="Z7" s="117"/>
-      <c r="AA7" s="117"/>
+      <c r="M7" s="109"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="109"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
+      <c r="S7" s="109"/>
+      <c r="T7" s="109"/>
+      <c r="U7" s="109"/>
+      <c r="V7" s="109"/>
+      <c r="W7" s="109"/>
+      <c r="X7" s="109"/>
+      <c r="Y7" s="109"/>
+      <c r="Z7" s="109"/>
+      <c r="AA7" s="109"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -3197,33 +3197,33 @@
     <row r="8" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32"/>
       <c r="B8" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="110"/>
+        <v>101</v>
+      </c>
+      <c r="C8" s="122"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="117"/>
-      <c r="P8" s="117"/>
-      <c r="Q8" s="117"/>
-      <c r="R8" s="117"/>
-      <c r="S8" s="117"/>
-      <c r="T8" s="117"/>
-      <c r="U8" s="117"/>
-      <c r="V8" s="117"/>
-      <c r="W8" s="117"/>
-      <c r="X8" s="117"/>
-      <c r="Y8" s="117"/>
-      <c r="Z8" s="117"/>
-      <c r="AA8" s="117"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="109"/>
+      <c r="Q8" s="109"/>
+      <c r="R8" s="109"/>
+      <c r="S8" s="109"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="109"/>
+      <c r="V8" s="109"/>
+      <c r="W8" s="109"/>
+      <c r="X8" s="109"/>
+      <c r="Y8" s="109"/>
+      <c r="Z8" s="109"/>
+      <c r="AA8" s="109"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -3233,31 +3233,31 @@
     <row r="9" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="113"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="127"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
-      <c r="M9" s="117"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
-      <c r="P9" s="117"/>
-      <c r="Q9" s="117"/>
-      <c r="R9" s="117"/>
-      <c r="S9" s="117"/>
-      <c r="T9" s="117"/>
-      <c r="U9" s="117"/>
-      <c r="V9" s="117"/>
-      <c r="W9" s="117"/>
-      <c r="X9" s="117"/>
-      <c r="Y9" s="117"/>
-      <c r="Z9" s="117"/>
-      <c r="AA9" s="117"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="109"/>
+      <c r="T9" s="109"/>
+      <c r="U9" s="109"/>
+      <c r="V9" s="109"/>
+      <c r="W9" s="109"/>
+      <c r="X9" s="109"/>
+      <c r="Y9" s="109"/>
+      <c r="Z9" s="109"/>
+      <c r="AA9" s="109"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -3277,21 +3277,21 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="117"/>
-      <c r="P10" s="117"/>
-      <c r="Q10" s="117"/>
-      <c r="R10" s="117"/>
-      <c r="S10" s="117"/>
-      <c r="T10" s="117"/>
-      <c r="U10" s="117"/>
-      <c r="V10" s="117"/>
-      <c r="W10" s="117"/>
-      <c r="X10" s="117"/>
-      <c r="Y10" s="117"/>
-      <c r="Z10" s="117"/>
-      <c r="AA10" s="117"/>
+      <c r="M10" s="109"/>
+      <c r="N10" s="109"/>
+      <c r="O10" s="109"/>
+      <c r="P10" s="109"/>
+      <c r="Q10" s="109"/>
+      <c r="R10" s="109"/>
+      <c r="S10" s="109"/>
+      <c r="T10" s="109"/>
+      <c r="U10" s="109"/>
+      <c r="V10" s="109"/>
+      <c r="W10" s="109"/>
+      <c r="X10" s="109"/>
+      <c r="Y10" s="109"/>
+      <c r="Z10" s="109"/>
+      <c r="AA10" s="109"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -3299,14 +3299,14 @@
       <c r="AF10" s="7"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="127" t="s">
-        <v>153</v>
+      <c r="A11" s="110" t="s">
+        <v>152</v>
       </c>
       <c r="B11" s="61"/>
       <c r="C11" s="62"/>
       <c r="D11" s="62"/>
       <c r="E11" s="74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="62"/>
       <c r="G11" s="62"/>
@@ -3315,21 +3315,21 @@
       <c r="J11" s="63"/>
       <c r="K11" s="64"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="117"/>
-      <c r="N11" s="117"/>
-      <c r="O11" s="117"/>
-      <c r="P11" s="117"/>
-      <c r="Q11" s="117"/>
-      <c r="R11" s="117"/>
-      <c r="S11" s="117"/>
-      <c r="T11" s="117"/>
-      <c r="U11" s="117"/>
-      <c r="V11" s="117"/>
-      <c r="W11" s="117"/>
-      <c r="X11" s="117"/>
-      <c r="Y11" s="117"/>
-      <c r="Z11" s="117"/>
-      <c r="AA11" s="117"/>
+      <c r="M11" s="109"/>
+      <c r="N11" s="109"/>
+      <c r="O11" s="109"/>
+      <c r="P11" s="109"/>
+      <c r="Q11" s="109"/>
+      <c r="R11" s="109"/>
+      <c r="S11" s="109"/>
+      <c r="T11" s="109"/>
+      <c r="U11" s="109"/>
+      <c r="V11" s="109"/>
+      <c r="W11" s="109"/>
+      <c r="X11" s="109"/>
+      <c r="Y11" s="109"/>
+      <c r="Z11" s="109"/>
+      <c r="AA11" s="109"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -3337,36 +3337,36 @@
       <c r="AF11" s="7"/>
     </row>
     <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="127"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="60"/>
       <c r="D12" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="114" t="s">
-        <v>124</v>
-      </c>
-      <c r="J12" s="114"/>
-      <c r="K12" s="115"/>
+      <c r="I12" s="128" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="128"/>
+      <c r="K12" s="129"/>
       <c r="L12" s="10"/>
-      <c r="M12" s="117"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="117"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="117"/>
-      <c r="R12" s="117"/>
-      <c r="S12" s="117"/>
-      <c r="T12" s="117"/>
-      <c r="U12" s="117"/>
-      <c r="V12" s="117"/>
-      <c r="W12" s="117"/>
-      <c r="X12" s="117"/>
-      <c r="Y12" s="117"/>
-      <c r="Z12" s="117"/>
-      <c r="AA12" s="117"/>
+      <c r="M12" s="109"/>
+      <c r="N12" s="109"/>
+      <c r="O12" s="109"/>
+      <c r="P12" s="109"/>
+      <c r="Q12" s="109"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="109"/>
+      <c r="T12" s="109"/>
+      <c r="U12" s="109"/>
+      <c r="V12" s="109"/>
+      <c r="W12" s="109"/>
+      <c r="X12" s="109"/>
+      <c r="Y12" s="109"/>
+      <c r="Z12" s="109"/>
+      <c r="AA12" s="109"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
@@ -3374,32 +3374,32 @@
       <c r="AF12" s="7"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="127"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="59"/>
       <c r="D13" s="9"/>
       <c r="E13" s="40"/>
       <c r="F13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="114"/>
-      <c r="J13" s="114"/>
-      <c r="K13" s="115"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="128"/>
+      <c r="K13" s="129"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="117"/>
-      <c r="R13" s="117"/>
-      <c r="S13" s="117"/>
-      <c r="T13" s="117"/>
-      <c r="U13" s="117"/>
-      <c r="V13" s="117"/>
-      <c r="W13" s="117"/>
-      <c r="X13" s="117"/>
-      <c r="Y13" s="117"/>
-      <c r="Z13" s="117"/>
-      <c r="AA13" s="117"/>
+      <c r="M13" s="109"/>
+      <c r="N13" s="109"/>
+      <c r="O13" s="109"/>
+      <c r="P13" s="109"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="109"/>
+      <c r="S13" s="109"/>
+      <c r="T13" s="109"/>
+      <c r="U13" s="109"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="109"/>
+      <c r="Y13" s="109"/>
+      <c r="Z13" s="109"/>
+      <c r="AA13" s="109"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
@@ -3407,7 +3407,7 @@
       <c r="AF13" s="7"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="127"/>
+      <c r="A14" s="110"/>
       <c r="B14" s="59"/>
       <c r="D14" s="9"/>
       <c r="E14" s="38"/>
@@ -3415,25 +3415,25 @@
         <v>41</v>
       </c>
       <c r="G14" s="12"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="114"/>
-      <c r="K14" s="115"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="129"/>
       <c r="L14" s="10"/>
-      <c r="M14" s="117"/>
-      <c r="N14" s="117"/>
-      <c r="O14" s="117"/>
-      <c r="P14" s="117"/>
-      <c r="Q14" s="117"/>
-      <c r="R14" s="117"/>
-      <c r="S14" s="117"/>
-      <c r="T14" s="117"/>
-      <c r="U14" s="117"/>
-      <c r="V14" s="117"/>
-      <c r="W14" s="117"/>
-      <c r="X14" s="117"/>
-      <c r="Y14" s="117"/>
-      <c r="Z14" s="117"/>
-      <c r="AA14" s="117"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="109"/>
+      <c r="O14" s="109"/>
+      <c r="P14" s="109"/>
+      <c r="Q14" s="109"/>
+      <c r="R14" s="109"/>
+      <c r="S14" s="109"/>
+      <c r="T14" s="109"/>
+      <c r="U14" s="109"/>
+      <c r="V14" s="109"/>
+      <c r="W14" s="109"/>
+      <c r="X14" s="109"/>
+      <c r="Y14" s="109"/>
+      <c r="Z14" s="109"/>
+      <c r="AA14" s="109"/>
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
       <c r="AD14" s="7"/>
@@ -3441,17 +3441,17 @@
       <c r="AF14" s="7"/>
     </row>
     <row r="15" spans="1:32" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="127"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="59"/>
       <c r="D15" s="28"/>
       <c r="E15" s="39"/>
       <c r="F15" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15" s="12"/>
-      <c r="I15" s="114"/>
-      <c r="J15" s="114"/>
-      <c r="K15" s="115"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="129"/>
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
       <c r="N15" s="29"/>
@@ -3475,15 +3475,15 @@
       <c r="AF15" s="7"/>
     </row>
     <row r="16" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="127"/>
+      <c r="A16" s="110"/>
       <c r="B16" s="59"/>
       <c r="D16" s="32"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="12"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="114"/>
-      <c r="K16" s="115"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="128"/>
+      <c r="K16" s="129"/>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
@@ -3507,19 +3507,19 @@
       <c r="AF16" s="7"/>
     </row>
     <row r="17" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="127"/>
+      <c r="A17" s="110"/>
       <c r="B17" s="59"/>
       <c r="D17" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17" s="41"/>
       <c r="F17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="G17" s="12"/>
-      <c r="I17" s="114"/>
-      <c r="J17" s="114"/>
-      <c r="K17" s="115"/>
+      <c r="I17" s="128"/>
+      <c r="J17" s="128"/>
+      <c r="K17" s="129"/>
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
@@ -3543,7 +3543,7 @@
       <c r="AF17" s="7"/>
     </row>
     <row r="18" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="127"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="59"/>
       <c r="D18" s="32"/>
       <c r="E18" s="11"/>
@@ -3574,10 +3574,10 @@
       <c r="AF18" s="7"/>
     </row>
     <row r="19" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="127"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="59"/>
       <c r="D19" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="11" t="s">
@@ -3585,32 +3585,32 @@
       </c>
       <c r="G19" s="12"/>
       <c r="J19" s="46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K19" s="47"/>
       <c r="L19" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M19" s="34"/>
       <c r="N19" s="50"/>
       <c r="O19" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P19" s="34"/>
       <c r="Q19" s="51"/>
       <c r="R19" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T19" s="55"/>
       <c r="U19" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V19" s="34"/>
       <c r="W19" s="57"/>
       <c r="X19" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y19" s="124"/>
+        <v>115</v>
+      </c>
+      <c r="Y19" s="86"/>
       <c r="Z19" s="66"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="7"/>
@@ -3620,36 +3620,36 @@
       <c r="AF19" s="7"/>
     </row>
     <row r="20" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="127"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="59"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="12"/>
       <c r="J20" s="78" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K20" s="48"/>
       <c r="L20" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M20" s="34"/>
       <c r="N20" s="54"/>
       <c r="O20" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P20" s="34"/>
       <c r="Q20" s="52"/>
       <c r="R20" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S20" s="34"/>
       <c r="V20" s="34"/>
       <c r="W20" s="58"/>
       <c r="X20" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y20" s="124"/>
+        <v>116</v>
+      </c>
+      <c r="Y20" s="86"/>
       <c r="Z20" s="66"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="7"/>
@@ -3659,38 +3659,38 @@
       <c r="AF20" s="7"/>
     </row>
     <row r="21" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="127"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="59"/>
       <c r="D21" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" s="45"/>
       <c r="F21" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G21" s="12"/>
       <c r="J21" s="78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K21" s="49"/>
       <c r="L21" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M21" s="34"/>
       <c r="P21" s="34"/>
       <c r="Q21" s="53"/>
       <c r="R21" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S21" s="34"/>
       <c r="T21" s="56"/>
       <c r="U21" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="V21" s="34"/>
       <c r="W21" s="34"/>
       <c r="X21" s="34"/>
-      <c r="Y21" s="124"/>
+      <c r="Y21" s="86"/>
       <c r="Z21" s="66"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="7"/>
@@ -3700,7 +3700,7 @@
       <c r="AF21" s="7"/>
     </row>
     <row r="22" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="127"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="67"/>
       <c r="C22" s="68"/>
       <c r="D22" s="69"/>
@@ -3735,31 +3735,31 @@
     </row>
     <row r="23" spans="1:32" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="82"/>
-      <c r="B23" s="125"/>
-      <c r="C23" s="125"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="83"/>
       <c r="E23" s="83"/>
-      <c r="F23" s="125"/>
+      <c r="F23" s="87"/>
       <c r="G23" s="12"/>
-      <c r="H23" s="126"/>
-      <c r="I23" s="126"/>
-      <c r="J23" s="124"/>
-      <c r="K23" s="124"/>
-      <c r="L23" s="124"/>
-      <c r="M23" s="124"/>
-      <c r="N23" s="124"/>
-      <c r="O23" s="124"/>
-      <c r="P23" s="124"/>
-      <c r="Q23" s="124"/>
-      <c r="R23" s="124"/>
-      <c r="S23" s="124"/>
-      <c r="T23" s="124"/>
-      <c r="U23" s="124"/>
-      <c r="V23" s="124"/>
-      <c r="W23" s="124"/>
-      <c r="X23" s="124"/>
-      <c r="Y23" s="124"/>
-      <c r="Z23" s="124"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
+      <c r="N23" s="86"/>
+      <c r="O23" s="86"/>
+      <c r="P23" s="86"/>
+      <c r="Q23" s="86"/>
+      <c r="R23" s="86"/>
+      <c r="S23" s="86"/>
+      <c r="T23" s="86"/>
+      <c r="U23" s="86"/>
+      <c r="V23" s="86"/>
+      <c r="W23" s="86"/>
+      <c r="X23" s="86"/>
+      <c r="Y23" s="86"/>
+      <c r="Z23" s="86"/>
       <c r="AA23" s="84"/>
       <c r="AB23" s="7"/>
       <c r="AC23" s="7"/>
@@ -3769,13 +3769,13 @@
     </row>
     <row r="24" spans="1:32" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="82"/>
-      <c r="B24" s="125"/>
-      <c r="C24" s="125"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
       <c r="D24" s="83"/>
       <c r="E24" s="61"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="134"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
@@ -3791,8 +3791,8 @@
       <c r="U24" s="63"/>
       <c r="V24" s="63"/>
       <c r="W24" s="64"/>
-      <c r="X24" s="124"/>
-      <c r="Y24" s="124"/>
+      <c r="X24" s="86"/>
+      <c r="Y24" s="86"/>
       <c r="Z24" s="84"/>
       <c r="AA24" s="7"/>
       <c r="AB24" s="7"/>
@@ -3801,38 +3801,38 @@
       <c r="AE24" s="7"/>
     </row>
     <row r="25" spans="1:32" s="85" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="132" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="135"/>
-      <c r="F25" s="126"/>
-      <c r="G25" s="125" t="s">
-        <v>154</v>
-      </c>
-      <c r="H25" s="128"/>
-      <c r="I25" s="125"/>
+      <c r="A25" s="93" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="96"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="87" t="s">
+        <v>153</v>
+      </c>
+      <c r="H25" s="89"/>
+      <c r="I25" s="87"/>
       <c r="J25" s="12"/>
-      <c r="K25" s="126"/>
-      <c r="L25" s="125" t="s">
+      <c r="K25" s="88"/>
+      <c r="L25" s="87" t="s">
+        <v>158</v>
+      </c>
+      <c r="M25" s="91"/>
+      <c r="N25" s="86"/>
+      <c r="O25" s="86"/>
+      <c r="P25" s="86"/>
+      <c r="Q25" s="87" t="s">
         <v>159</v>
       </c>
-      <c r="M25" s="130"/>
-      <c r="N25" s="124"/>
-      <c r="O25" s="124"/>
-      <c r="P25" s="124"/>
-      <c r="Q25" s="125" t="s">
+      <c r="R25" s="90"/>
+      <c r="S25" s="86"/>
+      <c r="T25" s="86"/>
+      <c r="U25" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="R25" s="129"/>
-      <c r="S25" s="124"/>
-      <c r="T25" s="124"/>
-      <c r="U25" s="125" t="s">
-        <v>161</v>
-      </c>
-      <c r="V25" s="131"/>
+      <c r="V25" s="92"/>
       <c r="W25" s="66"/>
-      <c r="X25" s="124"/>
-      <c r="Y25" s="124"/>
+      <c r="X25" s="86"/>
+      <c r="Y25" s="86"/>
       <c r="Z25" s="84"/>
       <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
@@ -3842,8 +3842,8 @@
     </row>
     <row r="26" spans="1:32" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="82"/>
-      <c r="B26" s="125"/>
-      <c r="C26" s="125"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="87"/>
       <c r="D26" s="83"/>
       <c r="E26" s="67"/>
       <c r="F26" s="70"/>
@@ -3864,8 +3864,8 @@
       <c r="U26" s="72"/>
       <c r="V26" s="72"/>
       <c r="W26" s="73"/>
-      <c r="X26" s="124"/>
-      <c r="Y26" s="124"/>
+      <c r="X26" s="86"/>
+      <c r="Y26" s="86"/>
       <c r="Z26" s="84"/>
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
@@ -3896,161 +3896,161 @@
       <c r="AF27" s="7"/>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A28" s="94" t="s">
+      <c r="A28" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="94"/>
-      <c r="C28" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="96"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="96"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="96"/>
-      <c r="N28" s="96"/>
-      <c r="O28" s="96"/>
-      <c r="P28" s="96"/>
-      <c r="Q28" s="96"/>
-      <c r="R28" s="96"/>
-      <c r="S28" s="96"/>
-      <c r="T28" s="96"/>
-      <c r="U28" s="96"/>
-      <c r="V28" s="96"/>
-      <c r="W28" s="96"/>
-      <c r="X28" s="96"/>
-      <c r="Y28" s="96"/>
-      <c r="Z28" s="96"/>
-      <c r="AA28" s="97"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="113"/>
+      <c r="J28" s="113"/>
+      <c r="K28" s="113"/>
+      <c r="L28" s="113"/>
+      <c r="M28" s="113"/>
+      <c r="N28" s="113"/>
+      <c r="O28" s="113"/>
+      <c r="P28" s="113"/>
+      <c r="Q28" s="113"/>
+      <c r="R28" s="113"/>
+      <c r="S28" s="113"/>
+      <c r="T28" s="113"/>
+      <c r="U28" s="113"/>
+      <c r="V28" s="113"/>
+      <c r="W28" s="113"/>
+      <c r="X28" s="113"/>
+      <c r="Y28" s="113"/>
+      <c r="Z28" s="113"/>
+      <c r="AA28" s="114"/>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
-      <c r="C29" s="98" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="99"/>
-      <c r="I29" s="99"/>
-      <c r="J29" s="99"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="99"/>
-      <c r="M29" s="99"/>
-      <c r="N29" s="99"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="99"/>
-      <c r="Q29" s="99"/>
-      <c r="R29" s="99"/>
-      <c r="S29" s="99"/>
-      <c r="T29" s="99"/>
-      <c r="U29" s="99"/>
-      <c r="V29" s="99"/>
-      <c r="W29" s="99"/>
-      <c r="X29" s="99"/>
-      <c r="Y29" s="99"/>
-      <c r="Z29" s="99"/>
-      <c r="AA29" s="100"/>
+      <c r="C29" s="115" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="116"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="116"/>
+      <c r="G29" s="116"/>
+      <c r="H29" s="116"/>
+      <c r="I29" s="116"/>
+      <c r="J29" s="116"/>
+      <c r="K29" s="116"/>
+      <c r="L29" s="116"/>
+      <c r="M29" s="116"/>
+      <c r="N29" s="116"/>
+      <c r="O29" s="116"/>
+      <c r="P29" s="116"/>
+      <c r="Q29" s="116"/>
+      <c r="R29" s="116"/>
+      <c r="S29" s="116"/>
+      <c r="T29" s="116"/>
+      <c r="U29" s="116"/>
+      <c r="V29" s="116"/>
+      <c r="W29" s="116"/>
+      <c r="X29" s="116"/>
+      <c r="Y29" s="116"/>
+      <c r="Z29" s="116"/>
+      <c r="AA29" s="117"/>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="99"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="99"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="99"/>
-      <c r="M30" s="99"/>
-      <c r="N30" s="99"/>
-      <c r="O30" s="99"/>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="99"/>
-      <c r="R30" s="99"/>
-      <c r="S30" s="99"/>
-      <c r="T30" s="99"/>
-      <c r="U30" s="99"/>
-      <c r="V30" s="99"/>
-      <c r="W30" s="99"/>
-      <c r="X30" s="99"/>
-      <c r="Y30" s="99"/>
-      <c r="Z30" s="99"/>
-      <c r="AA30" s="100"/>
+      <c r="C30" s="115" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="116"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="116"/>
+      <c r="G30" s="116"/>
+      <c r="H30" s="116"/>
+      <c r="I30" s="116"/>
+      <c r="J30" s="116"/>
+      <c r="K30" s="116"/>
+      <c r="L30" s="116"/>
+      <c r="M30" s="116"/>
+      <c r="N30" s="116"/>
+      <c r="O30" s="116"/>
+      <c r="P30" s="116"/>
+      <c r="Q30" s="116"/>
+      <c r="R30" s="116"/>
+      <c r="S30" s="116"/>
+      <c r="T30" s="116"/>
+      <c r="U30" s="116"/>
+      <c r="V30" s="116"/>
+      <c r="W30" s="116"/>
+      <c r="X30" s="116"/>
+      <c r="Y30" s="116"/>
+      <c r="Z30" s="116"/>
+      <c r="AA30" s="117"/>
     </row>
     <row r="31" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="101" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="102"/>
-      <c r="E31" s="102"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="102"/>
-      <c r="I31" s="102"/>
-      <c r="J31" s="102"/>
-      <c r="K31" s="102"/>
-      <c r="L31" s="102"/>
-      <c r="M31" s="102"/>
-      <c r="N31" s="102"/>
-      <c r="O31" s="102"/>
-      <c r="P31" s="102"/>
-      <c r="Q31" s="102"/>
-      <c r="R31" s="102"/>
-      <c r="S31" s="102"/>
-      <c r="T31" s="102"/>
-      <c r="U31" s="102"/>
-      <c r="V31" s="102"/>
-      <c r="W31" s="102"/>
-      <c r="X31" s="102"/>
-      <c r="Y31" s="102"/>
-      <c r="Z31" s="102"/>
-      <c r="AA31" s="103"/>
+      <c r="C31" s="118" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="119"/>
+      <c r="E31" s="119"/>
+      <c r="F31" s="119"/>
+      <c r="G31" s="119"/>
+      <c r="H31" s="119"/>
+      <c r="I31" s="119"/>
+      <c r="J31" s="119"/>
+      <c r="K31" s="119"/>
+      <c r="L31" s="119"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="119"/>
+      <c r="P31" s="119"/>
+      <c r="Q31" s="119"/>
+      <c r="R31" s="119"/>
+      <c r="S31" s="119"/>
+      <c r="T31" s="119"/>
+      <c r="U31" s="119"/>
+      <c r="V31" s="119"/>
+      <c r="W31" s="119"/>
+      <c r="X31" s="119"/>
+      <c r="Y31" s="119"/>
+      <c r="Z31" s="119"/>
+      <c r="AA31" s="120"/>
     </row>
     <row r="33" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="116"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="116"/>
-      <c r="E33" s="116"/>
-      <c r="F33" s="116"/>
-      <c r="G33" s="116"/>
-      <c r="H33" s="116"/>
-      <c r="I33" s="116"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="116"/>
-      <c r="L33" s="116"/>
-      <c r="M33" s="116"/>
-      <c r="N33" s="116"/>
-      <c r="O33" s="116"/>
-      <c r="P33" s="116"/>
-      <c r="Q33" s="116"/>
-      <c r="R33" s="116"/>
-      <c r="S33" s="116"/>
-      <c r="T33" s="116"/>
-      <c r="U33" s="116"/>
-      <c r="V33" s="116"/>
-      <c r="W33" s="116"/>
-      <c r="X33" s="116"/>
-      <c r="Y33" s="116"/>
-      <c r="Z33" s="116"/>
-      <c r="AA33" s="116"/>
+      <c r="B33" s="104"/>
+      <c r="C33" s="104"/>
+      <c r="D33" s="104"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="104"/>
+      <c r="I33" s="104"/>
+      <c r="J33" s="104"/>
+      <c r="K33" s="104"/>
+      <c r="L33" s="104"/>
+      <c r="M33" s="104"/>
+      <c r="N33" s="104"/>
+      <c r="O33" s="104"/>
+      <c r="P33" s="104"/>
+      <c r="Q33" s="104"/>
+      <c r="R33" s="104"/>
+      <c r="S33" s="104"/>
+      <c r="T33" s="104"/>
+      <c r="U33" s="104"/>
+      <c r="V33" s="104"/>
+      <c r="W33" s="104"/>
+      <c r="X33" s="104"/>
+      <c r="Y33" s="104"/>
+      <c r="Z33" s="104"/>
+      <c r="AA33" s="104"/>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -4475,10 +4475,10 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA44" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -4850,10 +4850,10 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="M56" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA56" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -4885,35 +4885,35 @@
       <c r="M59" s="10"/>
     </row>
     <row r="60" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="116" t="s">
+      <c r="A60" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="B60" s="116"/>
-      <c r="C60" s="116"/>
-      <c r="D60" s="116"/>
-      <c r="E60" s="116"/>
-      <c r="F60" s="116"/>
-      <c r="G60" s="116"/>
-      <c r="H60" s="116"/>
-      <c r="I60" s="116"/>
-      <c r="J60" s="116"/>
-      <c r="K60" s="116"/>
-      <c r="L60" s="116"/>
-      <c r="M60" s="116"/>
-      <c r="N60" s="116"/>
-      <c r="O60" s="116"/>
-      <c r="P60" s="116"/>
-      <c r="Q60" s="116"/>
-      <c r="R60" s="116"/>
-      <c r="S60" s="116"/>
-      <c r="T60" s="116"/>
-      <c r="U60" s="116"/>
-      <c r="V60" s="116"/>
-      <c r="W60" s="116"/>
-      <c r="X60" s="116"/>
-      <c r="Y60" s="116"/>
-      <c r="Z60" s="116"/>
-      <c r="AA60" s="116"/>
+      <c r="B60" s="104"/>
+      <c r="C60" s="104"/>
+      <c r="D60" s="104"/>
+      <c r="E60" s="104"/>
+      <c r="F60" s="104"/>
+      <c r="G60" s="104"/>
+      <c r="H60" s="104"/>
+      <c r="I60" s="104"/>
+      <c r="J60" s="104"/>
+      <c r="K60" s="104"/>
+      <c r="L60" s="104"/>
+      <c r="M60" s="104"/>
+      <c r="N60" s="104"/>
+      <c r="O60" s="104"/>
+      <c r="P60" s="104"/>
+      <c r="Q60" s="104"/>
+      <c r="R60" s="104"/>
+      <c r="S60" s="104"/>
+      <c r="T60" s="104"/>
+      <c r="U60" s="104"/>
+      <c r="V60" s="104"/>
+      <c r="W60" s="104"/>
+      <c r="X60" s="104"/>
+      <c r="Y60" s="104"/>
+      <c r="Z60" s="104"/>
+      <c r="AA60" s="104"/>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -5668,16 +5668,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A33:AA33"/>
-    <mergeCell ref="A60:AA60"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="M3:AA14"/>
-    <mergeCell ref="A11:A22"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C28:AA28"/>
@@ -5691,6 +5681,16 @@
     <mergeCell ref="C29:AA29"/>
     <mergeCell ref="C8:G9"/>
     <mergeCell ref="I12:K17"/>
+    <mergeCell ref="A33:AA33"/>
+    <mergeCell ref="A60:AA60"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="M3:AA14"/>
+    <mergeCell ref="A11:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -5714,20 +5714,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
+      <c r="A1" s="111" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -5746,35 +5746,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="94"/>
+      <c r="B3" s="108"/>
       <c r="C3" s="105"/>
       <c r="D3" s="106"/>
       <c r="E3" s="106"/>
       <c r="F3" s="106"/>
       <c r="G3" s="107"/>
-      <c r="J3" s="94" t="s">
+      <c r="J3" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="117"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="117"/>
-      <c r="AA3" s="117"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -5782,35 +5782,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="94"/>
+      <c r="B4" s="108"/>
       <c r="C4" s="105"/>
       <c r="D4" s="106"/>
       <c r="E4" s="106"/>
       <c r="F4" s="106"/>
       <c r="G4" s="107"/>
-      <c r="J4" s="94" t="s">
+      <c r="J4" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="117"/>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="117"/>
-      <c r="U4" s="117"/>
-      <c r="V4" s="117"/>
-      <c r="W4" s="117"/>
-      <c r="X4" s="117"/>
-      <c r="Y4" s="117"/>
-      <c r="Z4" s="117"/>
-      <c r="AA4" s="117"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109"/>
+      <c r="X4" s="109"/>
+      <c r="Y4" s="109"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -5819,26 +5819,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="104" t="s">
+      <c r="J5" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
-      <c r="Y5" s="117"/>
-      <c r="Z5" s="117"/>
-      <c r="AA5" s="117"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="109"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="109"/>
+      <c r="Z5" s="109"/>
+      <c r="AA5" s="109"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -5846,30 +5846,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="105"/>
       <c r="D6" s="106"/>
       <c r="E6" s="106"/>
       <c r="F6" s="106"/>
       <c r="G6" s="107"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="117"/>
-      <c r="U6" s="117"/>
-      <c r="V6" s="117"/>
-      <c r="W6" s="117"/>
-      <c r="X6" s="117"/>
-      <c r="Y6" s="117"/>
-      <c r="Z6" s="117"/>
-      <c r="AA6" s="117"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="109"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="109"/>
+      <c r="V6" s="109"/>
+      <c r="W6" s="109"/>
+      <c r="X6" s="109"/>
+      <c r="Y6" s="109"/>
+      <c r="Z6" s="109"/>
+      <c r="AA6" s="109"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -5877,30 +5877,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="94"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="105"/>
       <c r="D7" s="106"/>
       <c r="E7" s="106"/>
       <c r="F7" s="106"/>
       <c r="G7" s="107"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117"/>
-      <c r="Q7" s="117"/>
-      <c r="R7" s="117"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="117"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="117"/>
-      <c r="X7" s="117"/>
-      <c r="Y7" s="117"/>
-      <c r="Z7" s="117"/>
-      <c r="AA7" s="117"/>
+      <c r="M7" s="109"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="109"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
+      <c r="S7" s="109"/>
+      <c r="T7" s="109"/>
+      <c r="U7" s="109"/>
+      <c r="V7" s="109"/>
+      <c r="W7" s="109"/>
+      <c r="X7" s="109"/>
+      <c r="Y7" s="109"/>
+      <c r="Z7" s="109"/>
+      <c r="AA7" s="109"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -5910,33 +5910,33 @@
     <row r="8" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32"/>
       <c r="B8" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="110"/>
+        <v>101</v>
+      </c>
+      <c r="C8" s="122"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="117"/>
-      <c r="P8" s="117"/>
-      <c r="Q8" s="117"/>
-      <c r="R8" s="117"/>
-      <c r="S8" s="117"/>
-      <c r="T8" s="117"/>
-      <c r="U8" s="117"/>
-      <c r="V8" s="117"/>
-      <c r="W8" s="117"/>
-      <c r="X8" s="117"/>
-      <c r="Y8" s="117"/>
-      <c r="Z8" s="117"/>
-      <c r="AA8" s="117"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="109"/>
+      <c r="Q8" s="109"/>
+      <c r="R8" s="109"/>
+      <c r="S8" s="109"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="109"/>
+      <c r="V8" s="109"/>
+      <c r="W8" s="109"/>
+      <c r="X8" s="109"/>
+      <c r="Y8" s="109"/>
+      <c r="Z8" s="109"/>
+      <c r="AA8" s="109"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -5946,31 +5946,31 @@
     <row r="9" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="113"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="127"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
-      <c r="M9" s="117"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
-      <c r="P9" s="117"/>
-      <c r="Q9" s="117"/>
-      <c r="R9" s="117"/>
-      <c r="S9" s="117"/>
-      <c r="T9" s="117"/>
-      <c r="U9" s="117"/>
-      <c r="V9" s="117"/>
-      <c r="W9" s="117"/>
-      <c r="X9" s="117"/>
-      <c r="Y9" s="117"/>
-      <c r="Z9" s="117"/>
-      <c r="AA9" s="117"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="109"/>
+      <c r="T9" s="109"/>
+      <c r="U9" s="109"/>
+      <c r="V9" s="109"/>
+      <c r="W9" s="109"/>
+      <c r="X9" s="109"/>
+      <c r="Y9" s="109"/>
+      <c r="Z9" s="109"/>
+      <c r="AA9" s="109"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -5985,21 +5985,21 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="117"/>
-      <c r="P10" s="117"/>
-      <c r="Q10" s="117"/>
-      <c r="R10" s="117"/>
-      <c r="S10" s="117"/>
-      <c r="T10" s="117"/>
-      <c r="U10" s="117"/>
-      <c r="V10" s="117"/>
-      <c r="W10" s="117"/>
-      <c r="X10" s="117"/>
-      <c r="Y10" s="117"/>
-      <c r="Z10" s="117"/>
-      <c r="AA10" s="117"/>
+      <c r="M10" s="109"/>
+      <c r="N10" s="109"/>
+      <c r="O10" s="109"/>
+      <c r="P10" s="109"/>
+      <c r="Q10" s="109"/>
+      <c r="R10" s="109"/>
+      <c r="S10" s="109"/>
+      <c r="T10" s="109"/>
+      <c r="U10" s="109"/>
+      <c r="V10" s="109"/>
+      <c r="W10" s="109"/>
+      <c r="X10" s="109"/>
+      <c r="Y10" s="109"/>
+      <c r="Z10" s="109"/>
+      <c r="AA10" s="109"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -6009,27 +6009,27 @@
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="M11" s="117"/>
-      <c r="N11" s="117"/>
-      <c r="O11" s="117"/>
-      <c r="P11" s="117"/>
-      <c r="Q11" s="117"/>
-      <c r="R11" s="117"/>
-      <c r="S11" s="117"/>
-      <c r="T11" s="117"/>
-      <c r="U11" s="117"/>
-      <c r="V11" s="117"/>
-      <c r="W11" s="117"/>
-      <c r="X11" s="117"/>
-      <c r="Y11" s="117"/>
-      <c r="Z11" s="117"/>
-      <c r="AA11" s="117"/>
+        <v>132</v>
+      </c>
+      <c r="M11" s="109"/>
+      <c r="N11" s="109"/>
+      <c r="O11" s="109"/>
+      <c r="P11" s="109"/>
+      <c r="Q11" s="109"/>
+      <c r="R11" s="109"/>
+      <c r="S11" s="109"/>
+      <c r="T11" s="109"/>
+      <c r="U11" s="109"/>
+      <c r="V11" s="109"/>
+      <c r="W11" s="109"/>
+      <c r="X11" s="109"/>
+      <c r="Y11" s="109"/>
+      <c r="Z11" s="109"/>
+      <c r="AA11" s="109"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -6042,23 +6042,23 @@
       <c r="D12" s="13"/>
       <c r="E12" s="43"/>
       <c r="F12" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="M12" s="117"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="117"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="117"/>
-      <c r="R12" s="117"/>
-      <c r="S12" s="117"/>
-      <c r="T12" s="117"/>
-      <c r="U12" s="117"/>
-      <c r="V12" s="117"/>
-      <c r="W12" s="117"/>
-      <c r="X12" s="117"/>
-      <c r="Y12" s="117"/>
-      <c r="Z12" s="117"/>
-      <c r="AA12" s="117"/>
+        <v>133</v>
+      </c>
+      <c r="M12" s="109"/>
+      <c r="N12" s="109"/>
+      <c r="O12" s="109"/>
+      <c r="P12" s="109"/>
+      <c r="Q12" s="109"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="109"/>
+      <c r="T12" s="109"/>
+      <c r="U12" s="109"/>
+      <c r="V12" s="109"/>
+      <c r="W12" s="109"/>
+      <c r="X12" s="109"/>
+      <c r="Y12" s="109"/>
+      <c r="Z12" s="109"/>
+      <c r="AA12" s="109"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
@@ -6072,26 +6072,26 @@
       <c r="D13" s="11"/>
       <c r="E13" s="44"/>
       <c r="F13" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="117"/>
-      <c r="R13" s="117"/>
-      <c r="S13" s="117"/>
-      <c r="T13" s="117"/>
-      <c r="U13" s="117"/>
-      <c r="V13" s="117"/>
-      <c r="W13" s="117"/>
-      <c r="X13" s="117"/>
-      <c r="Y13" s="117"/>
-      <c r="Z13" s="117"/>
-      <c r="AA13" s="117"/>
+      <c r="M13" s="109"/>
+      <c r="N13" s="109"/>
+      <c r="O13" s="109"/>
+      <c r="P13" s="109"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="109"/>
+      <c r="S13" s="109"/>
+      <c r="T13" s="109"/>
+      <c r="U13" s="109"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="109"/>
+      <c r="Y13" s="109"/>
+      <c r="Z13" s="109"/>
+      <c r="AA13" s="109"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
@@ -6105,7 +6105,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="41"/>
       <c r="F14" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -6141,7 +6141,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="36"/>
       <c r="F15" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -6192,161 +6192,161 @@
       <c r="AF16" s="7"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="94" t="s">
+      <c r="A17" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="94"/>
-      <c r="C17" s="95" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
-      <c r="S17" s="96"/>
-      <c r="T17" s="96"/>
-      <c r="U17" s="96"/>
-      <c r="V17" s="96"/>
-      <c r="W17" s="96"/>
-      <c r="X17" s="96"/>
-      <c r="Y17" s="96"/>
-      <c r="Z17" s="96"/>
-      <c r="AA17" s="97"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="112" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="113"/>
+      <c r="J17" s="113"/>
+      <c r="K17" s="113"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="113"/>
+      <c r="N17" s="113"/>
+      <c r="O17" s="113"/>
+      <c r="P17" s="113"/>
+      <c r="Q17" s="113"/>
+      <c r="R17" s="113"/>
+      <c r="S17" s="113"/>
+      <c r="T17" s="113"/>
+      <c r="U17" s="113"/>
+      <c r="V17" s="113"/>
+      <c r="W17" s="113"/>
+      <c r="X17" s="113"/>
+      <c r="Y17" s="113"/>
+      <c r="Z17" s="113"/>
+      <c r="AA17" s="114"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
-      <c r="C18" s="98" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="99"/>
-      <c r="J18" s="99"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="99"/>
-      <c r="M18" s="99"/>
-      <c r="N18" s="99"/>
-      <c r="O18" s="99"/>
-      <c r="P18" s="99"/>
-      <c r="Q18" s="99"/>
-      <c r="R18" s="99"/>
-      <c r="S18" s="99"/>
-      <c r="T18" s="99"/>
-      <c r="U18" s="99"/>
-      <c r="V18" s="99"/>
-      <c r="W18" s="99"/>
-      <c r="X18" s="99"/>
-      <c r="Y18" s="99"/>
-      <c r="Z18" s="99"/>
-      <c r="AA18" s="100"/>
+      <c r="C18" s="115" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="116"/>
+      <c r="E18" s="116"/>
+      <c r="F18" s="116"/>
+      <c r="G18" s="116"/>
+      <c r="H18" s="116"/>
+      <c r="I18" s="116"/>
+      <c r="J18" s="116"/>
+      <c r="K18" s="116"/>
+      <c r="L18" s="116"/>
+      <c r="M18" s="116"/>
+      <c r="N18" s="116"/>
+      <c r="O18" s="116"/>
+      <c r="P18" s="116"/>
+      <c r="Q18" s="116"/>
+      <c r="R18" s="116"/>
+      <c r="S18" s="116"/>
+      <c r="T18" s="116"/>
+      <c r="U18" s="116"/>
+      <c r="V18" s="116"/>
+      <c r="W18" s="116"/>
+      <c r="X18" s="116"/>
+      <c r="Y18" s="116"/>
+      <c r="Z18" s="116"/>
+      <c r="AA18" s="117"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
-      <c r="C19" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="99"/>
-      <c r="E19" s="99"/>
-      <c r="F19" s="99"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="99"/>
-      <c r="J19" s="99"/>
-      <c r="K19" s="99"/>
-      <c r="L19" s="99"/>
-      <c r="M19" s="99"/>
-      <c r="N19" s="99"/>
-      <c r="O19" s="99"/>
-      <c r="P19" s="99"/>
-      <c r="Q19" s="99"/>
-      <c r="R19" s="99"/>
-      <c r="S19" s="99"/>
-      <c r="T19" s="99"/>
-      <c r="U19" s="99"/>
-      <c r="V19" s="99"/>
-      <c r="W19" s="99"/>
-      <c r="X19" s="99"/>
-      <c r="Y19" s="99"/>
-      <c r="Z19" s="99"/>
-      <c r="AA19" s="100"/>
+      <c r="C19" s="115" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="116"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="116"/>
+      <c r="I19" s="116"/>
+      <c r="J19" s="116"/>
+      <c r="K19" s="116"/>
+      <c r="L19" s="116"/>
+      <c r="M19" s="116"/>
+      <c r="N19" s="116"/>
+      <c r="O19" s="116"/>
+      <c r="P19" s="116"/>
+      <c r="Q19" s="116"/>
+      <c r="R19" s="116"/>
+      <c r="S19" s="116"/>
+      <c r="T19" s="116"/>
+      <c r="U19" s="116"/>
+      <c r="V19" s="116"/>
+      <c r="W19" s="116"/>
+      <c r="X19" s="116"/>
+      <c r="Y19" s="116"/>
+      <c r="Z19" s="116"/>
+      <c r="AA19" s="117"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
-      <c r="C20" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="102"/>
-      <c r="E20" s="102"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="102"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="102"/>
-      <c r="L20" s="102"/>
-      <c r="M20" s="102"/>
-      <c r="N20" s="102"/>
-      <c r="O20" s="102"/>
-      <c r="P20" s="102"/>
-      <c r="Q20" s="102"/>
-      <c r="R20" s="102"/>
-      <c r="S20" s="102"/>
-      <c r="T20" s="102"/>
-      <c r="U20" s="102"/>
-      <c r="V20" s="102"/>
-      <c r="W20" s="102"/>
-      <c r="X20" s="102"/>
-      <c r="Y20" s="102"/>
-      <c r="Z20" s="102"/>
-      <c r="AA20" s="103"/>
+      <c r="C20" s="118" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="119"/>
+      <c r="E20" s="119"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="119"/>
+      <c r="H20" s="119"/>
+      <c r="I20" s="119"/>
+      <c r="J20" s="119"/>
+      <c r="K20" s="119"/>
+      <c r="L20" s="119"/>
+      <c r="M20" s="119"/>
+      <c r="N20" s="119"/>
+      <c r="O20" s="119"/>
+      <c r="P20" s="119"/>
+      <c r="Q20" s="119"/>
+      <c r="R20" s="119"/>
+      <c r="S20" s="119"/>
+      <c r="T20" s="119"/>
+      <c r="U20" s="119"/>
+      <c r="V20" s="119"/>
+      <c r="W20" s="119"/>
+      <c r="X20" s="119"/>
+      <c r="Y20" s="119"/>
+      <c r="Z20" s="119"/>
+      <c r="AA20" s="120"/>
     </row>
     <row r="22" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="116"/>
-      <c r="J22" s="116"/>
-      <c r="K22" s="116"/>
-      <c r="L22" s="116"/>
-      <c r="M22" s="116"/>
-      <c r="N22" s="116"/>
-      <c r="O22" s="116"/>
-      <c r="P22" s="116"/>
-      <c r="Q22" s="116"/>
-      <c r="R22" s="116"/>
-      <c r="S22" s="116"/>
-      <c r="T22" s="116"/>
-      <c r="U22" s="116"/>
-      <c r="V22" s="116"/>
-      <c r="W22" s="116"/>
-      <c r="X22" s="116"/>
-      <c r="Y22" s="116"/>
-      <c r="Z22" s="116"/>
-      <c r="AA22" s="116"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="104"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="104"/>
+      <c r="O22" s="104"/>
+      <c r="P22" s="104"/>
+      <c r="Q22" s="104"/>
+      <c r="R22" s="104"/>
+      <c r="S22" s="104"/>
+      <c r="T22" s="104"/>
+      <c r="U22" s="104"/>
+      <c r="V22" s="104"/>
+      <c r="W22" s="104"/>
+      <c r="X22" s="104"/>
+      <c r="Y22" s="104"/>
+      <c r="Z22" s="104"/>
+      <c r="AA22" s="104"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -7145,35 +7145,35 @@
       <c r="J46" s="19"/>
     </row>
     <row r="49" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="116" t="s">
-        <v>89</v>
-      </c>
-      <c r="B49" s="116"/>
-      <c r="C49" s="116"/>
-      <c r="D49" s="116"/>
-      <c r="E49" s="116"/>
-      <c r="F49" s="116"/>
-      <c r="G49" s="116"/>
-      <c r="H49" s="116"/>
-      <c r="I49" s="116"/>
-      <c r="J49" s="116"/>
-      <c r="K49" s="116"/>
-      <c r="L49" s="116"/>
-      <c r="M49" s="116"/>
-      <c r="N49" s="116"/>
-      <c r="O49" s="116"/>
-      <c r="P49" s="116"/>
-      <c r="Q49" s="116"/>
-      <c r="R49" s="116"/>
-      <c r="S49" s="116"/>
-      <c r="T49" s="116"/>
-      <c r="U49" s="116"/>
-      <c r="V49" s="116"/>
-      <c r="W49" s="116"/>
-      <c r="X49" s="116"/>
-      <c r="Y49" s="116"/>
-      <c r="Z49" s="116"/>
-      <c r="AA49" s="116"/>
+      <c r="A49" s="104" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="104"/>
+      <c r="C49" s="104"/>
+      <c r="D49" s="104"/>
+      <c r="E49" s="104"/>
+      <c r="F49" s="104"/>
+      <c r="G49" s="104"/>
+      <c r="H49" s="104"/>
+      <c r="I49" s="104"/>
+      <c r="J49" s="104"/>
+      <c r="K49" s="104"/>
+      <c r="L49" s="104"/>
+      <c r="M49" s="104"/>
+      <c r="N49" s="104"/>
+      <c r="O49" s="104"/>
+      <c r="P49" s="104"/>
+      <c r="Q49" s="104"/>
+      <c r="R49" s="104"/>
+      <c r="S49" s="104"/>
+      <c r="T49" s="104"/>
+      <c r="U49" s="104"/>
+      <c r="V49" s="104"/>
+      <c r="W49" s="104"/>
+      <c r="X49" s="104"/>
+      <c r="Y49" s="104"/>
+      <c r="Z49" s="104"/>
+      <c r="AA49" s="104"/>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -7920,16 +7920,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:AA13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="C19:AA19"/>
     <mergeCell ref="C20:AA20"/>
     <mergeCell ref="A22:AA22"/>
@@ -7941,6 +7931,16 @@
     <mergeCell ref="C17:AA17"/>
     <mergeCell ref="C18:AA18"/>
     <mergeCell ref="C8:G9"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:AA13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7964,20 +7964,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
+      <c r="A1" s="111" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -7993,32 +7993,32 @@
       <c r="AC2" s="7"/>
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="94"/>
+      <c r="B3" s="108"/>
       <c r="C3" s="105"/>
       <c r="D3" s="106"/>
       <c r="E3" s="106"/>
       <c r="F3" s="106"/>
       <c r="G3" s="107"/>
-      <c r="J3" s="94" t="s">
+      <c r="J3" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="117"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
@@ -8026,32 +8026,32 @@
       <c r="AC3" s="7"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="94"/>
+      <c r="B4" s="108"/>
       <c r="C4" s="105"/>
       <c r="D4" s="106"/>
       <c r="E4" s="106"/>
       <c r="F4" s="106"/>
       <c r="G4" s="107"/>
-      <c r="J4" s="94" t="s">
+      <c r="J4" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="117"/>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="117"/>
-      <c r="U4" s="117"/>
-      <c r="V4" s="117"/>
-      <c r="W4" s="117"/>
-      <c r="X4" s="117"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109"/>
+      <c r="X4" s="109"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
@@ -8060,21 +8060,21 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="109"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
@@ -8082,27 +8082,27 @@
       <c r="AC5" s="7"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="105"/>
       <c r="D6" s="106"/>
       <c r="E6" s="106"/>
       <c r="F6" s="106"/>
       <c r="G6" s="107"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="117"/>
-      <c r="U6" s="117"/>
-      <c r="V6" s="117"/>
-      <c r="W6" s="117"/>
-      <c r="X6" s="117"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="109"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="109"/>
+      <c r="V6" s="109"/>
+      <c r="W6" s="109"/>
+      <c r="X6" s="109"/>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
@@ -8110,27 +8110,27 @@
       <c r="AC6" s="7"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="94"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="105"/>
       <c r="D7" s="106"/>
       <c r="E7" s="106"/>
       <c r="F7" s="106"/>
       <c r="G7" s="107"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117"/>
-      <c r="Q7" s="117"/>
-      <c r="R7" s="117"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="117"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="117"/>
-      <c r="X7" s="117"/>
+      <c r="M7" s="109"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="109"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
+      <c r="S7" s="109"/>
+      <c r="T7" s="109"/>
+      <c r="U7" s="109"/>
+      <c r="V7" s="109"/>
+      <c r="W7" s="109"/>
+      <c r="X7" s="109"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="7"/>
@@ -8140,30 +8140,30 @@
     <row r="8" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32"/>
       <c r="B8" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="110"/>
+        <v>101</v>
+      </c>
+      <c r="C8" s="122"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="117"/>
-      <c r="P8" s="117"/>
-      <c r="Q8" s="117"/>
-      <c r="R8" s="117"/>
-      <c r="S8" s="117"/>
-      <c r="T8" s="117"/>
-      <c r="U8" s="117"/>
-      <c r="V8" s="117"/>
-      <c r="W8" s="117"/>
-      <c r="X8" s="117"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="109"/>
+      <c r="Q8" s="109"/>
+      <c r="R8" s="109"/>
+      <c r="S8" s="109"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="109"/>
+      <c r="V8" s="109"/>
+      <c r="W8" s="109"/>
+      <c r="X8" s="109"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
@@ -8173,28 +8173,28 @@
     <row r="9" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="113"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="127"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
-      <c r="M9" s="117"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
-      <c r="P9" s="117"/>
-      <c r="Q9" s="117"/>
-      <c r="R9" s="117"/>
-      <c r="S9" s="117"/>
-      <c r="T9" s="117"/>
-      <c r="U9" s="117"/>
-      <c r="V9" s="117"/>
-      <c r="W9" s="117"/>
-      <c r="X9" s="117"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="109"/>
+      <c r="T9" s="109"/>
+      <c r="U9" s="109"/>
+      <c r="V9" s="109"/>
+      <c r="W9" s="109"/>
+      <c r="X9" s="109"/>
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="7"/>
@@ -8209,18 +8209,18 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="117"/>
-      <c r="P10" s="117"/>
-      <c r="Q10" s="117"/>
-      <c r="R10" s="117"/>
-      <c r="S10" s="117"/>
-      <c r="T10" s="117"/>
-      <c r="U10" s="117"/>
-      <c r="V10" s="117"/>
-      <c r="W10" s="117"/>
-      <c r="X10" s="117"/>
+      <c r="M10" s="109"/>
+      <c r="N10" s="109"/>
+      <c r="O10" s="109"/>
+      <c r="P10" s="109"/>
+      <c r="Q10" s="109"/>
+      <c r="R10" s="109"/>
+      <c r="S10" s="109"/>
+      <c r="T10" s="109"/>
+      <c r="U10" s="109"/>
+      <c r="V10" s="109"/>
+      <c r="W10" s="109"/>
+      <c r="X10" s="109"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="7"/>
@@ -8230,24 +8230,24 @@
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="D11" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="M11" s="117"/>
-      <c r="N11" s="117"/>
-      <c r="O11" s="117"/>
-      <c r="P11" s="117"/>
-      <c r="Q11" s="117"/>
-      <c r="R11" s="117"/>
-      <c r="S11" s="117"/>
-      <c r="T11" s="117"/>
-      <c r="U11" s="117"/>
-      <c r="V11" s="117"/>
-      <c r="W11" s="117"/>
-      <c r="X11" s="117"/>
+        <v>128</v>
+      </c>
+      <c r="M11" s="109"/>
+      <c r="N11" s="109"/>
+      <c r="O11" s="109"/>
+      <c r="P11" s="109"/>
+      <c r="Q11" s="109"/>
+      <c r="R11" s="109"/>
+      <c r="S11" s="109"/>
+      <c r="T11" s="109"/>
+      <c r="U11" s="109"/>
+      <c r="V11" s="109"/>
+      <c r="W11" s="109"/>
+      <c r="X11" s="109"/>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
@@ -8260,20 +8260,20 @@
       <c r="D12" s="13"/>
       <c r="E12" s="79"/>
       <c r="F12" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="M12" s="117"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="117"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="117"/>
-      <c r="R12" s="117"/>
-      <c r="S12" s="117"/>
-      <c r="T12" s="117"/>
-      <c r="U12" s="117"/>
-      <c r="V12" s="117"/>
-      <c r="W12" s="117"/>
-      <c r="X12" s="117"/>
+        <v>129</v>
+      </c>
+      <c r="M12" s="109"/>
+      <c r="N12" s="109"/>
+      <c r="O12" s="109"/>
+      <c r="P12" s="109"/>
+      <c r="Q12" s="109"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="109"/>
+      <c r="T12" s="109"/>
+      <c r="U12" s="109"/>
+      <c r="V12" s="109"/>
+      <c r="W12" s="109"/>
+      <c r="X12" s="109"/>
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
@@ -8287,22 +8287,22 @@
       <c r="D13" s="11"/>
       <c r="E13" s="24"/>
       <c r="F13" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="117"/>
-      <c r="R13" s="117"/>
-      <c r="S13" s="117"/>
-      <c r="T13" s="117"/>
-      <c r="U13" s="117"/>
-      <c r="V13" s="117"/>
-      <c r="W13" s="117"/>
-      <c r="X13" s="117"/>
+      <c r="M13" s="109"/>
+      <c r="N13" s="109"/>
+      <c r="O13" s="109"/>
+      <c r="P13" s="109"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="109"/>
+      <c r="S13" s="109"/>
+      <c r="T13" s="109"/>
+      <c r="U13" s="109"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="109"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
@@ -8328,325 +8328,383 @@
       <c r="AC14" s="7"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="95" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="96"/>
-      <c r="H15" s="96"/>
-      <c r="I15" s="96"/>
-      <c r="J15" s="96"/>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="96"/>
-      <c r="O15" s="96"/>
-      <c r="P15" s="96"/>
-      <c r="Q15" s="96"/>
-      <c r="R15" s="96"/>
-      <c r="S15" s="96"/>
-      <c r="T15" s="96"/>
-      <c r="U15" s="96"/>
-      <c r="V15" s="96"/>
-      <c r="W15" s="96"/>
-      <c r="X15" s="97"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="112" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="113"/>
+      <c r="M15" s="113"/>
+      <c r="N15" s="113"/>
+      <c r="O15" s="113"/>
+      <c r="P15" s="113"/>
+      <c r="Q15" s="113"/>
+      <c r="R15" s="113"/>
+      <c r="S15" s="113"/>
+      <c r="T15" s="113"/>
+      <c r="U15" s="113"/>
+      <c r="V15" s="113"/>
+      <c r="W15" s="113"/>
+      <c r="X15" s="114"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
-      <c r="C16" s="98" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="99"/>
-      <c r="O16" s="99"/>
-      <c r="P16" s="99"/>
-      <c r="Q16" s="99"/>
-      <c r="R16" s="99"/>
-      <c r="S16" s="99"/>
-      <c r="T16" s="99"/>
-      <c r="U16" s="99"/>
-      <c r="V16" s="99"/>
-      <c r="W16" s="99"/>
-      <c r="X16" s="100"/>
+      <c r="C16" s="115" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="116"/>
+      <c r="K16" s="116"/>
+      <c r="L16" s="116"/>
+      <c r="M16" s="116"/>
+      <c r="N16" s="116"/>
+      <c r="O16" s="116"/>
+      <c r="P16" s="116"/>
+      <c r="Q16" s="116"/>
+      <c r="R16" s="116"/>
+      <c r="S16" s="116"/>
+      <c r="T16" s="116"/>
+      <c r="U16" s="116"/>
+      <c r="V16" s="116"/>
+      <c r="W16" s="116"/>
+      <c r="X16" s="117"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
-      <c r="C17" s="101" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="102"/>
-      <c r="E17" s="102"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="102"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="102"/>
-      <c r="L17" s="102"/>
-      <c r="M17" s="102"/>
-      <c r="N17" s="102"/>
-      <c r="O17" s="102"/>
-      <c r="P17" s="102"/>
-      <c r="Q17" s="102"/>
-      <c r="R17" s="102"/>
-      <c r="S17" s="102"/>
-      <c r="T17" s="102"/>
-      <c r="U17" s="102"/>
-      <c r="V17" s="102"/>
-      <c r="W17" s="102"/>
-      <c r="X17" s="103"/>
+      <c r="C17" s="118" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="119"/>
+      <c r="E17" s="119"/>
+      <c r="F17" s="119"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="119"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="119"/>
+      <c r="T17" s="119"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="120"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="134" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="D19" s="134"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="134" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="119"/>
-      <c r="E19" s="119"/>
-      <c r="F19" s="119"/>
-      <c r="G19" s="119" t="s">
+      <c r="H19" s="134"/>
+      <c r="I19" s="134" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" s="134"/>
+      <c r="K19" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="H19" s="119"/>
-      <c r="I19" s="119" t="s">
+      <c r="L19" s="134" t="s">
+        <v>119</v>
+      </c>
+      <c r="M19" s="134"/>
+      <c r="N19" s="134" t="s">
         <v>121</v>
       </c>
-      <c r="J19" s="119"/>
-      <c r="K19" s="26" t="s">
+      <c r="O19" s="134"/>
+      <c r="P19" s="134" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q19" s="134"/>
+      <c r="R19" s="131" t="s">
         <v>97</v>
       </c>
-      <c r="L19" s="119" t="s">
-        <v>120</v>
-      </c>
-      <c r="M19" s="119"/>
-      <c r="N19" s="119" t="s">
-        <v>122</v>
-      </c>
-      <c r="O19" s="119"/>
-      <c r="P19" s="119" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q19" s="119"/>
-      <c r="R19" s="121" t="s">
-        <v>98</v>
-      </c>
-      <c r="S19" s="121"/>
-      <c r="T19" s="121"/>
-      <c r="U19" s="121"/>
-      <c r="V19" s="121"/>
-      <c r="W19" s="121"/>
-      <c r="X19" s="121"/>
+      <c r="S19" s="131"/>
+      <c r="T19" s="131"/>
+      <c r="U19" s="131"/>
+      <c r="V19" s="131"/>
+      <c r="W19" s="131"/>
+      <c r="X19" s="131"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>1</v>
       </c>
-      <c r="C20" s="118"/>
-      <c r="D20" s="118"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="120"/>
-      <c r="J20" s="120"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="130"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="135"/>
+      <c r="J20" s="135"/>
       <c r="K20" s="37"/>
-      <c r="L20" s="118"/>
-      <c r="M20" s="118"/>
-      <c r="N20" s="120"/>
-      <c r="O20" s="120"/>
-      <c r="P20" s="120"/>
-      <c r="Q20" s="120"/>
-      <c r="R20" s="122"/>
-      <c r="S20" s="122"/>
-      <c r="T20" s="122"/>
-      <c r="U20" s="122"/>
-      <c r="V20" s="122"/>
-      <c r="W20" s="122"/>
-      <c r="X20" s="122"/>
+      <c r="L20" s="130"/>
+      <c r="M20" s="130"/>
+      <c r="N20" s="135"/>
+      <c r="O20" s="135"/>
+      <c r="P20" s="135"/>
+      <c r="Q20" s="135"/>
+      <c r="R20" s="132"/>
+      <c r="S20" s="132"/>
+      <c r="T20" s="132"/>
+      <c r="U20" s="132"/>
+      <c r="V20" s="132"/>
+      <c r="W20" s="132"/>
+      <c r="X20" s="132"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>2</v>
       </c>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="130"/>
+      <c r="E21" s="130"/>
+      <c r="F21" s="130"/>
+      <c r="G21" s="130"/>
+      <c r="H21" s="130"/>
+      <c r="I21" s="130"/>
+      <c r="J21" s="130"/>
       <c r="K21" s="37"/>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
-      <c r="N21" s="118"/>
-      <c r="O21" s="118"/>
-      <c r="P21" s="118"/>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="123"/>
-      <c r="S21" s="123"/>
-      <c r="T21" s="123"/>
-      <c r="U21" s="123"/>
-      <c r="V21" s="123"/>
-      <c r="W21" s="123"/>
-      <c r="X21" s="123"/>
+      <c r="L21" s="130"/>
+      <c r="M21" s="130"/>
+      <c r="N21" s="130"/>
+      <c r="O21" s="130"/>
+      <c r="P21" s="130"/>
+      <c r="Q21" s="130"/>
+      <c r="R21" s="133"/>
+      <c r="S21" s="133"/>
+      <c r="T21" s="133"/>
+      <c r="U21" s="133"/>
+      <c r="V21" s="133"/>
+      <c r="W21" s="133"/>
+      <c r="X21" s="133"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>3</v>
       </c>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="118"/>
+      <c r="C22" s="130"/>
+      <c r="D22" s="130"/>
+      <c r="E22" s="130"/>
+      <c r="F22" s="130"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="130"/>
+      <c r="I22" s="130"/>
+      <c r="J22" s="130"/>
       <c r="K22" s="37"/>
-      <c r="L22" s="118"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="118"/>
-      <c r="P22" s="118"/>
-      <c r="Q22" s="118"/>
-      <c r="R22" s="123"/>
-      <c r="S22" s="123"/>
-      <c r="T22" s="123"/>
-      <c r="U22" s="123"/>
-      <c r="V22" s="123"/>
-      <c r="W22" s="123"/>
-      <c r="X22" s="123"/>
+      <c r="L22" s="130"/>
+      <c r="M22" s="130"/>
+      <c r="N22" s="130"/>
+      <c r="O22" s="130"/>
+      <c r="P22" s="130"/>
+      <c r="Q22" s="130"/>
+      <c r="R22" s="133"/>
+      <c r="S22" s="133"/>
+      <c r="T22" s="133"/>
+      <c r="U22" s="133"/>
+      <c r="V22" s="133"/>
+      <c r="W22" s="133"/>
+      <c r="X22" s="133"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>4</v>
       </c>
-      <c r="C23" s="118"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
-      <c r="J23" s="118"/>
+      <c r="C23" s="130"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="130"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="130"/>
+      <c r="I23" s="130"/>
+      <c r="J23" s="130"/>
       <c r="K23" s="37"/>
-      <c r="L23" s="118"/>
-      <c r="M23" s="118"/>
-      <c r="N23" s="118"/>
-      <c r="O23" s="118"/>
-      <c r="P23" s="118"/>
-      <c r="Q23" s="118"/>
-      <c r="R23" s="123"/>
-      <c r="S23" s="123"/>
-      <c r="T23" s="123"/>
-      <c r="U23" s="123"/>
-      <c r="V23" s="123"/>
-      <c r="W23" s="123"/>
-      <c r="X23" s="123"/>
+      <c r="L23" s="130"/>
+      <c r="M23" s="130"/>
+      <c r="N23" s="130"/>
+      <c r="O23" s="130"/>
+      <c r="P23" s="130"/>
+      <c r="Q23" s="130"/>
+      <c r="R23" s="133"/>
+      <c r="S23" s="133"/>
+      <c r="T23" s="133"/>
+      <c r="U23" s="133"/>
+      <c r="V23" s="133"/>
+      <c r="W23" s="133"/>
+      <c r="X23" s="133"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>5</v>
       </c>
-      <c r="C24" s="118"/>
-      <c r="D24" s="118"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="118"/>
-      <c r="J24" s="118"/>
+      <c r="C24" s="130"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="130"/>
+      <c r="H24" s="130"/>
+      <c r="I24" s="130"/>
+      <c r="J24" s="130"/>
       <c r="K24" s="37"/>
-      <c r="L24" s="118"/>
-      <c r="M24" s="118"/>
-      <c r="N24" s="118"/>
-      <c r="O24" s="118"/>
-      <c r="P24" s="118"/>
-      <c r="Q24" s="118"/>
-      <c r="R24" s="123"/>
-      <c r="S24" s="123"/>
-      <c r="T24" s="123"/>
-      <c r="U24" s="123"/>
-      <c r="V24" s="123"/>
-      <c r="W24" s="123"/>
-      <c r="X24" s="123"/>
+      <c r="L24" s="130"/>
+      <c r="M24" s="130"/>
+      <c r="N24" s="130"/>
+      <c r="O24" s="130"/>
+      <c r="P24" s="130"/>
+      <c r="Q24" s="130"/>
+      <c r="R24" s="133"/>
+      <c r="S24" s="133"/>
+      <c r="T24" s="133"/>
+      <c r="U24" s="133"/>
+      <c r="V24" s="133"/>
+      <c r="W24" s="133"/>
+      <c r="X24" s="133"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>6</v>
       </c>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="118"/>
-      <c r="F25" s="118"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="118"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="118"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="130"/>
       <c r="K25" s="37"/>
-      <c r="L25" s="118"/>
-      <c r="M25" s="118"/>
-      <c r="N25" s="118"/>
-      <c r="O25" s="118"/>
-      <c r="P25" s="118"/>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="123"/>
-      <c r="S25" s="123"/>
-      <c r="T25" s="123"/>
-      <c r="U25" s="123"/>
-      <c r="V25" s="123"/>
-      <c r="W25" s="123"/>
-      <c r="X25" s="123"/>
+      <c r="L25" s="130"/>
+      <c r="M25" s="130"/>
+      <c r="N25" s="130"/>
+      <c r="O25" s="130"/>
+      <c r="P25" s="130"/>
+      <c r="Q25" s="130"/>
+      <c r="R25" s="133"/>
+      <c r="S25" s="133"/>
+      <c r="T25" s="133"/>
+      <c r="U25" s="133"/>
+      <c r="V25" s="133"/>
+      <c r="W25" s="133"/>
+      <c r="X25" s="133"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="118"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="118"/>
+      <c r="C26" s="130"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="130"/>
+      <c r="H26" s="130"/>
+      <c r="I26" s="130"/>
+      <c r="J26" s="130"/>
       <c r="K26" s="37"/>
-      <c r="L26" s="118"/>
-      <c r="M26" s="118"/>
-      <c r="N26" s="118"/>
-      <c r="O26" s="118"/>
-      <c r="P26" s="118"/>
-      <c r="Q26" s="118"/>
-      <c r="R26" s="123"/>
-      <c r="S26" s="123"/>
-      <c r="T26" s="123"/>
-      <c r="U26" s="123"/>
-      <c r="V26" s="123"/>
-      <c r="W26" s="123"/>
-      <c r="X26" s="123"/>
+      <c r="L26" s="130"/>
+      <c r="M26" s="130"/>
+      <c r="N26" s="130"/>
+      <c r="O26" s="130"/>
+      <c r="P26" s="130"/>
+      <c r="Q26" s="130"/>
+      <c r="R26" s="133"/>
+      <c r="S26" s="133"/>
+      <c r="T26" s="133"/>
+      <c r="U26" s="133"/>
+      <c r="V26" s="133"/>
+      <c r="W26" s="133"/>
+      <c r="X26" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C16:X16"/>
+    <mergeCell ref="C17:X17"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C15:X15"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:X13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C8:G9"/>
     <mergeCell ref="P24:Q24"/>
     <mergeCell ref="P25:Q25"/>
     <mergeCell ref="P26:Q26"/>
@@ -8663,64 +8721,6 @@
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="P22:Q22"/>
     <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:X13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C8:G9"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C16:X16"/>
-    <mergeCell ref="C17:X17"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C15:X15"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8746,20 +8746,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
+      <c r="A1" s="111" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -8778,35 +8778,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="94"/>
+      <c r="B3" s="108"/>
       <c r="C3" s="105"/>
       <c r="D3" s="106"/>
       <c r="E3" s="106"/>
       <c r="F3" s="106"/>
       <c r="G3" s="107"/>
-      <c r="J3" s="94" t="s">
+      <c r="J3" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="117"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="117"/>
-      <c r="AA3" s="117"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -8814,35 +8814,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="94"/>
+      <c r="B4" s="108"/>
       <c r="C4" s="105"/>
       <c r="D4" s="106"/>
       <c r="E4" s="106"/>
       <c r="F4" s="106"/>
       <c r="G4" s="107"/>
-      <c r="J4" s="94" t="s">
+      <c r="J4" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="117"/>
-      <c r="P4" s="117"/>
-      <c r="Q4" s="117"/>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="117"/>
-      <c r="U4" s="117"/>
-      <c r="V4" s="117"/>
-      <c r="W4" s="117"/>
-      <c r="X4" s="117"/>
-      <c r="Y4" s="117"/>
-      <c r="Z4" s="117"/>
-      <c r="AA4" s="117"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="109"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="109"/>
+      <c r="X4" s="109"/>
+      <c r="Y4" s="109"/>
+      <c r="Z4" s="109"/>
+      <c r="AA4" s="109"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -8851,26 +8851,26 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="104" t="s">
+      <c r="J5" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
-      <c r="Y5" s="117"/>
-      <c r="Z5" s="117"/>
-      <c r="AA5" s="117"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="109"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="109"/>
+      <c r="Z5" s="109"/>
+      <c r="AA5" s="109"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -8878,30 +8878,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="105"/>
       <c r="D6" s="106"/>
       <c r="E6" s="106"/>
       <c r="F6" s="106"/>
       <c r="G6" s="107"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
-      <c r="Q6" s="117"/>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="117"/>
-      <c r="U6" s="117"/>
-      <c r="V6" s="117"/>
-      <c r="W6" s="117"/>
-      <c r="X6" s="117"/>
-      <c r="Y6" s="117"/>
-      <c r="Z6" s="117"/>
-      <c r="AA6" s="117"/>
+      <c r="M6" s="109"/>
+      <c r="N6" s="109"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
+      <c r="R6" s="109"/>
+      <c r="S6" s="109"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="109"/>
+      <c r="V6" s="109"/>
+      <c r="W6" s="109"/>
+      <c r="X6" s="109"/>
+      <c r="Y6" s="109"/>
+      <c r="Z6" s="109"/>
+      <c r="AA6" s="109"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -8909,30 +8909,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="94"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="105"/>
       <c r="D7" s="106"/>
       <c r="E7" s="106"/>
       <c r="F7" s="106"/>
       <c r="G7" s="107"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117"/>
-      <c r="Q7" s="117"/>
-      <c r="R7" s="117"/>
-      <c r="S7" s="117"/>
-      <c r="T7" s="117"/>
-      <c r="U7" s="117"/>
-      <c r="V7" s="117"/>
-      <c r="W7" s="117"/>
-      <c r="X7" s="117"/>
-      <c r="Y7" s="117"/>
-      <c r="Z7" s="117"/>
-      <c r="AA7" s="117"/>
+      <c r="M7" s="109"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="109"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
+      <c r="S7" s="109"/>
+      <c r="T7" s="109"/>
+      <c r="U7" s="109"/>
+      <c r="V7" s="109"/>
+      <c r="W7" s="109"/>
+      <c r="X7" s="109"/>
+      <c r="Y7" s="109"/>
+      <c r="Z7" s="109"/>
+      <c r="AA7" s="109"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -8942,33 +8942,33 @@
     <row r="8" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32"/>
       <c r="B8" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="110"/>
+        <v>101</v>
+      </c>
+      <c r="C8" s="122"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="117"/>
-      <c r="P8" s="117"/>
-      <c r="Q8" s="117"/>
-      <c r="R8" s="117"/>
-      <c r="S8" s="117"/>
-      <c r="T8" s="117"/>
-      <c r="U8" s="117"/>
-      <c r="V8" s="117"/>
-      <c r="W8" s="117"/>
-      <c r="X8" s="117"/>
-      <c r="Y8" s="117"/>
-      <c r="Z8" s="117"/>
-      <c r="AA8" s="117"/>
+      <c r="M8" s="109"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="109"/>
+      <c r="Q8" s="109"/>
+      <c r="R8" s="109"/>
+      <c r="S8" s="109"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="109"/>
+      <c r="V8" s="109"/>
+      <c r="W8" s="109"/>
+      <c r="X8" s="109"/>
+      <c r="Y8" s="109"/>
+      <c r="Z8" s="109"/>
+      <c r="AA8" s="109"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -8978,31 +8978,31 @@
     <row r="9" spans="1:32" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="111"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="113"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="127"/>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
-      <c r="M9" s="117"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
-      <c r="P9" s="117"/>
-      <c r="Q9" s="117"/>
-      <c r="R9" s="117"/>
-      <c r="S9" s="117"/>
-      <c r="T9" s="117"/>
-      <c r="U9" s="117"/>
-      <c r="V9" s="117"/>
-      <c r="W9" s="117"/>
-      <c r="X9" s="117"/>
-      <c r="Y9" s="117"/>
-      <c r="Z9" s="117"/>
-      <c r="AA9" s="117"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="109"/>
+      <c r="T9" s="109"/>
+      <c r="U9" s="109"/>
+      <c r="V9" s="109"/>
+      <c r="W9" s="109"/>
+      <c r="X9" s="109"/>
+      <c r="Y9" s="109"/>
+      <c r="Z9" s="109"/>
+      <c r="AA9" s="109"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
@@ -9017,21 +9017,21 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="117"/>
-      <c r="P10" s="117"/>
-      <c r="Q10" s="117"/>
-      <c r="R10" s="117"/>
-      <c r="S10" s="117"/>
-      <c r="T10" s="117"/>
-      <c r="U10" s="117"/>
-      <c r="V10" s="117"/>
-      <c r="W10" s="117"/>
-      <c r="X10" s="117"/>
-      <c r="Y10" s="117"/>
-      <c r="Z10" s="117"/>
-      <c r="AA10" s="117"/>
+      <c r="M10" s="109"/>
+      <c r="N10" s="109"/>
+      <c r="O10" s="109"/>
+      <c r="P10" s="109"/>
+      <c r="Q10" s="109"/>
+      <c r="R10" s="109"/>
+      <c r="S10" s="109"/>
+      <c r="T10" s="109"/>
+      <c r="U10" s="109"/>
+      <c r="V10" s="109"/>
+      <c r="W10" s="109"/>
+      <c r="X10" s="109"/>
+      <c r="Y10" s="109"/>
+      <c r="Z10" s="109"/>
+      <c r="AA10" s="109"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
@@ -9041,7 +9041,7 @@
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="C11" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="105"/>
       <c r="E11" s="106"/>
@@ -9049,21 +9049,21 @@
       <c r="G11" s="106"/>
       <c r="H11" s="106"/>
       <c r="I11" s="107"/>
-      <c r="M11" s="117"/>
-      <c r="N11" s="117"/>
-      <c r="O11" s="117"/>
-      <c r="P11" s="117"/>
-      <c r="Q11" s="117"/>
-      <c r="R11" s="117"/>
-      <c r="S11" s="117"/>
-      <c r="T11" s="117"/>
-      <c r="U11" s="117"/>
-      <c r="V11" s="117"/>
-      <c r="W11" s="117"/>
-      <c r="X11" s="117"/>
-      <c r="Y11" s="117"/>
-      <c r="Z11" s="117"/>
-      <c r="AA11" s="117"/>
+      <c r="M11" s="109"/>
+      <c r="N11" s="109"/>
+      <c r="O11" s="109"/>
+      <c r="P11" s="109"/>
+      <c r="Q11" s="109"/>
+      <c r="R11" s="109"/>
+      <c r="S11" s="109"/>
+      <c r="T11" s="109"/>
+      <c r="U11" s="109"/>
+      <c r="V11" s="109"/>
+      <c r="W11" s="109"/>
+      <c r="X11" s="109"/>
+      <c r="Y11" s="109"/>
+      <c r="Z11" s="109"/>
+      <c r="AA11" s="109"/>
       <c r="AB11" s="7"/>
       <c r="AC11" s="7"/>
       <c r="AD11" s="7"/>
@@ -9073,21 +9073,21 @@
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
-      <c r="M12" s="117"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="117"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="117"/>
-      <c r="R12" s="117"/>
-      <c r="S12" s="117"/>
-      <c r="T12" s="117"/>
-      <c r="U12" s="117"/>
-      <c r="V12" s="117"/>
-      <c r="W12" s="117"/>
-      <c r="X12" s="117"/>
-      <c r="Y12" s="117"/>
-      <c r="Z12" s="117"/>
-      <c r="AA12" s="117"/>
+      <c r="M12" s="109"/>
+      <c r="N12" s="109"/>
+      <c r="O12" s="109"/>
+      <c r="P12" s="109"/>
+      <c r="Q12" s="109"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="109"/>
+      <c r="T12" s="109"/>
+      <c r="U12" s="109"/>
+      <c r="V12" s="109"/>
+      <c r="W12" s="109"/>
+      <c r="X12" s="109"/>
+      <c r="Y12" s="109"/>
+      <c r="Z12" s="109"/>
+      <c r="AA12" s="109"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
@@ -9098,29 +9098,29 @@
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="23"/>
       <c r="H13" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I13" s="105"/>
       <c r="J13" s="107"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="117"/>
-      <c r="R13" s="117"/>
-      <c r="S13" s="117"/>
-      <c r="T13" s="117"/>
-      <c r="U13" s="117"/>
-      <c r="V13" s="117"/>
-      <c r="W13" s="117"/>
-      <c r="X13" s="117"/>
-      <c r="Y13" s="117"/>
-      <c r="Z13" s="117"/>
-      <c r="AA13" s="117"/>
+      <c r="M13" s="109"/>
+      <c r="N13" s="109"/>
+      <c r="O13" s="109"/>
+      <c r="P13" s="109"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="109"/>
+      <c r="S13" s="109"/>
+      <c r="T13" s="109"/>
+      <c r="U13" s="109"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="109"/>
+      <c r="Y13" s="109"/>
+      <c r="Z13" s="109"/>
+      <c r="AA13" s="109"/>
       <c r="AB13" s="7"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
@@ -9152,11 +9152,11 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C15" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="23"/>
       <c r="H15" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I15" s="105"/>
       <c r="J15" s="107"/>
@@ -9165,23 +9165,17 @@
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="23"/>
       <c r="H17" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="105"/>
       <c r="J17" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="J3:L3"/>
     <mergeCell ref="M3:AA13"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:G4"/>
@@ -9194,6 +9188,12 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G9"/>
     <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="J3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>